<commit_message>
createCssAnimation, isCssLengthProperty, px, throwError
</commit_message>
<xml_diff>
--- a/misc/fit-rect-aspect-ratio-calc.xlsx
+++ b/misc/fit-rect-aspect-ratio-calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelneff/projects/utik/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D950FAD0-4D6D-B946-8FD3-6EE06040D454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ED6163-B3FA-4941-A0BD-FA7BC2B6D291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="19880" xr2:uid="{549C457E-A7E6-294A-AF87-A5A5B8B840AA}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>